<commit_message>
Upgrade Java Libraries and migrating Log4j
</commit_message>
<xml_diff>
--- a/adrezo/help/ressource/adrezo_modele_csv.xlsx
+++ b/adrezo/help/ressource/adrezo_modele_csv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Adrezo_CSV" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
     </ext>
   </extLst>
 </workbook>
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
     <comment ref="A5" authorId="0">
@@ -34,7 +34,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Utiliser le nom du contexte</t>
+          <t>Utiliser le nom du contexte</t>
         </r>
       </text>
     </comment>
@@ -47,7 +47,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Utiliser le nom du site</t>
+          <t>Utiliser le nom du site</t>
         </r>
       </text>
     </comment>
@@ -60,7 +60,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Utiliser le nom du sous-réseau</t>
+          <t>Utiliser le nom du sous-réseau</t>
         </r>
       </text>
     </comment>
@@ -73,7 +73,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Masque de sous-réseau = Nombre de 2 à 32</t>
+          <t>Masque de sous-réseau = Nombre de 2 à 32</t>
         </r>
       </text>
     </comment>
@@ -86,7 +86,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Limité à 20 caractères</t>
+          <t>Limité à 20 caractères</t>
         </r>
       </text>
     </comment>
@@ -99,7 +99,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Limité à 100 caractères</t>
+          <t>Limité à 100 caractères</t>
         </r>
       </text>
     </comment>
@@ -112,7 +112,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Format sans séparateur. Exemple : 2A695B6325EF</t>
+          <t>Format sans séparateur. Exemple : 2A695B6325EF</t>
         </r>
       </text>
     </comment>
@@ -125,7 +125,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Entrer les 4 parties de l'adresse IP en nombre normal, la colonne résultat contiendra l'IP au bon format</t>
+          <t>Entrer les 4 parties de l'adresse IP en nombre normal, la colonne résultat contiendra l'IP au bon format</t>
         </r>
       </text>
     </comment>
@@ -136,58 +136,58 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
-    <t xml:space="preserve">DETAILS DANS LES COMMENTAIRES DES ENTETES DE COLONNES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recopier les formules des colonnes L et N a chaque ligne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Obligatoire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non Obligatoire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contexte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sous-Réseau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masque</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libellé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresse MAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresse IP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partie 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partie 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partie 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résultat</t>
+    <t>DETAILS DANS LES COMMENTAIRES DES ENTETES DE COLONNES</t>
+  </si>
+  <si>
+    <t>Recopier les formules des colonnes L et N a chaque ligne</t>
+  </si>
+  <si>
+    <t>Obligatoire</t>
+  </si>
+  <si>
+    <t>Non Obligatoire</t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>Contexte</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Sous-Réseau</t>
+  </si>
+  <si>
+    <t>Masque</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Libellé</t>
+  </si>
+  <si>
+    <t>Adresse MAC</t>
+  </si>
+  <si>
+    <t>Adresse IP</t>
+  </si>
+  <si>
+    <t>Partie 1</t>
+  </si>
+  <si>
+    <t>Partie 2</t>
+  </si>
+  <si>
+    <t>Partie 3</t>
+  </si>
+  <si>
+    <t>Partie 4</t>
+  </si>
+  <si>
+    <t>Résultat</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -423,23 +423,23 @@
   </sheetPr>
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="1" width="12.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="85.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="12.7"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2091836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="8" style="1" width="12.6989795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.6989795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="85.8163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="12.6989795918367"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,7 +582,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>